<commit_message>
Finished changes Aug 10
</commit_message>
<xml_diff>
--- a/data_aug4/SO-PackExport Data_1013888.xlsx
+++ b/data_aug4/SO-PackExport Data_1013888.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\data_aug4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0491FBD1-BFA1-43E5-8CDB-FE359CC9B402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E447FEA-740E-4726-80C3-F1456B646E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
   <si>
     <t>OrderType</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>Touch Up Pen for Beechwood &amp; Rock Elm Finishes</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
   <dimension ref="A1:AP68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1315,7 +1318,9 @@
       <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>75</v>
       </c>
@@ -1553,7 +1558,9 @@
       <c r="E9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>77</v>
       </c>

</xml_diff>